<commit_message>
Add About page explanation for choice in potential
</commit_message>
<xml_diff>
--- a/InputData/geoeng/ERWD/Enhanced Rock Weathering Data.xlsx
+++ b/InputData/geoeng/ERWD/Enhanced Rock Weathering Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\geoeng\ERWD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EEFD6F9-AC62-4988-8549-5C72F21AA390}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98AAF143-D02D-4BA9-A61C-1E4CE8806B97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,6 @@
     <sheet name="ERWD-capex" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -62,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Sources:</t>
   </si>
@@ -167,6 +166,18 @@
   </si>
   <si>
     <t>ERWD Enhanced Rock Weathering Amortized CapEx and OM</t>
+  </si>
+  <si>
+    <t>Because enhanced rock weathering involves the crushing of rock and application</t>
+  </si>
+  <si>
+    <t>on fields, which are available technologies today, we assume the full potential</t>
+  </si>
+  <si>
+    <t>could be realized as soon as 2030. However, it is worth noting that would require</t>
+  </si>
+  <si>
+    <t>a very large scale-up of capacity and transportation logistics.</t>
   </si>
 </sst>
 </file>
@@ -586,16 +597,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.85546875" customWidth="1"/>
-    <col min="2" max="2" width="47.140625" customWidth="1"/>
+    <col min="2" max="2" width="53" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -656,36 +667,56 @@
         <v>25</v>
       </c>
     </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>35</v>
+      </c>
+    </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>19</v>
+      <c r="A16" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
         <v>0.88711067149387013</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>31</v>
       </c>
-      <c r="B23">
+      <c r="B27">
         <v>947817</v>
       </c>
     </row>
@@ -1120,7 +1151,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="6">
-        <f>'Fuhrman data'!B4*About!B23</f>
+        <f>'Fuhrman data'!B4*About!B27</f>
         <v>625559.22</v>
       </c>
       <c r="C2" s="6">
@@ -2250,7 +2281,7 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <f>('Fuhrman data'!B1+'Fuhrman data'!B2)*About!A21</f>
+        <f>('Fuhrman data'!B1+'Fuhrman data'!B2)*About!A25</f>
         <v>255.4878733902346</v>
       </c>
       <c r="C2">
@@ -2370,7 +2401,7 @@
         <v>137.14730981295241</v>
       </c>
       <c r="AF2">
-        <f>'Fuhrman data'!B1*About!A21</f>
+        <f>'Fuhrman data'!B1*About!A25</f>
         <v>133.06660072408053</v>
       </c>
     </row>

</xml_diff>